<commit_message>
updated with new DWR data
and stop/start time file
</commit_message>
<xml_diff>
--- a/Processing/raw/SondeData_StartStopTimes.xlsx
+++ b/Processing/raw/SondeData_StartStopTimes.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater.sharepoint.com/sites/dwr-frpa/Water Quality Lab/Data Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{B256B240-512B-48C1-BE10-D4EE7FC48F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED583366-A0E2-468A-AA9B-4A15990D4498}"/>
+  <xr:revisionPtr revIDLastSave="646" documentId="8_{B256B240-512B-48C1-BE10-D4EE7FC48F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A56AD40-0D28-45BC-996D-8B9206485C41}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="9320" windowHeight="10800" tabRatio="875" firstSheet="1" activeTab="4" xr2:uid="{7D31225D-82AC-49F7-AF21-28358DF8E574}"/>
+    <workbookView xWindow="10300" yWindow="0" windowWidth="8900" windowHeight="10800" tabRatio="875" activeTab="3" xr2:uid="{7D31225D-82AC-49F7-AF21-28358DF8E574}"/>
   </bookViews>
   <sheets>
-    <sheet name="ARN" sheetId="1" r:id="rId1"/>
-    <sheet name="BRD" sheetId="2" r:id="rId2"/>
-    <sheet name="TRB" sheetId="4" r:id="rId3"/>
+    <sheet name="ReadMe" sheetId="11" r:id="rId1"/>
+    <sheet name="ARN" sheetId="1" r:id="rId2"/>
+    <sheet name="BRD" sheetId="2" r:id="rId3"/>
     <sheet name="TRM" sheetId="10" r:id="rId4"/>
     <sheet name="TRC" sheetId="6" r:id="rId5"/>
     <sheet name="WNG" sheetId="7" r:id="rId6"/>
     <sheet name="WNT" sheetId="8" r:id="rId7"/>
     <sheet name="LYR" sheetId="3" r:id="rId8"/>
-    <sheet name="TRDock" sheetId="5" r:id="rId9"/>
-    <sheet name="YFF" sheetId="9" r:id="rId10"/>
+    <sheet name="LYS" sheetId="9" r:id="rId9"/>
+    <sheet name="TRDock" sheetId="5" r:id="rId10"/>
+    <sheet name="TRB-Retired" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="72">
   <si>
     <t>Field Sheet</t>
   </si>
@@ -204,6 +205,63 @@
   </si>
   <si>
     <t>TRM</t>
+  </si>
+  <si>
+    <t>Cutting Notes:</t>
+  </si>
+  <si>
+    <t>Data File Start Time</t>
+  </si>
+  <si>
+    <t>Data File End Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-should be prior to Arrival Time </t>
+  </si>
+  <si>
+    <t>- should always be at least one 15-minute interval after Departure Time</t>
+  </si>
+  <si>
+    <t>Arrival Time</t>
+  </si>
+  <si>
+    <t>Dept Time</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>LYR</t>
+  </si>
+  <si>
+    <t>LYS</t>
+  </si>
+  <si>
+    <t>first TAL sensor install</t>
+  </si>
+  <si>
+    <t>THR-24</t>
+  </si>
+  <si>
+    <t>THR-23</t>
+  </si>
+  <si>
+    <t>Buoy cleaning; No exchange; Expect weird readings during this time</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>Chlor sensor installed</t>
+  </si>
+  <si>
+    <t>1015(ish)</t>
+  </si>
+  <si>
+    <t>1000(ish)</t>
+  </si>
+  <si>
+    <t>MISSING DATA FILE</t>
   </si>
 </sst>
 </file>
@@ -259,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -272,6 +330,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,10 +346,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -589,517 +644,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6D3776-44C9-402D-8899-CF36CF41AF68}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76492402-3033-45FE-943C-940199001B63}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44758</v>
-      </c>
-      <c r="C3">
-        <v>1335</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44772</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>44434</v>
-      </c>
-      <c r="C5">
-        <v>1010</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>44483</v>
-      </c>
-      <c r="C6">
-        <v>1145</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>44519</v>
-      </c>
-      <c r="C7">
-        <v>1125</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44547</v>
-      </c>
-      <c r="C8">
-        <v>1041</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
-        <v>44577</v>
-      </c>
-      <c r="C9">
-        <v>1150</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>44621</v>
-      </c>
-      <c r="C10">
-        <v>1250</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44658</v>
-      </c>
-      <c r="C11">
-        <v>1218</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44700</v>
-      </c>
-      <c r="C12">
-        <v>1015</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44742</v>
-      </c>
-      <c r="C13">
-        <v>910</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44775</v>
-      </c>
-      <c r="C14">
-        <v>1039</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>1041</v>
-      </c>
-      <c r="G14">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1">
-        <v>44817</v>
-      </c>
-      <c r="C15">
-        <v>1145</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>1145</v>
-      </c>
-      <c r="G15">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1">
-        <v>44845</v>
-      </c>
-      <c r="C16">
-        <v>1204</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16">
-        <v>1200</v>
-      </c>
-      <c r="G16">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1">
-        <v>44882</v>
-      </c>
-      <c r="C17">
-        <v>1401</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17">
-        <v>1400</v>
-      </c>
-      <c r="G17">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3">
-        <v>44915</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18">
-        <v>1245</v>
-      </c>
-      <c r="G18">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="1">
-        <v>44959</v>
-      </c>
-      <c r="C19">
-        <v>1230</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19">
-        <v>1245</v>
-      </c>
-      <c r="G19">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45002</v>
-      </c>
-      <c r="C20">
-        <v>1218</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>1230</v>
-      </c>
-      <c r="G20">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1">
-        <v>45049</v>
-      </c>
-      <c r="C21">
-        <v>1317</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21">
-        <v>1330</v>
-      </c>
-      <c r="G21">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="1">
-        <v>45083</v>
-      </c>
-      <c r="C22">
-        <v>1044</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22">
-        <v>1200</v>
-      </c>
-      <c r="G22">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="1">
-        <v>45120</v>
-      </c>
-      <c r="C23">
-        <v>1207</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23">
-        <v>1215</v>
-      </c>
-      <c r="G23">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="1">
-        <v>45147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAB0EEE-8947-4168-BA23-5BDB3B3C4A39}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E61B50-78AE-4051-9DCA-CE85349BDC81}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="H1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F002B337-BF1C-4A03-9136-9E55E40FA3F2}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +775,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1136,6 +799,53 @@
       </c>
       <c r="H2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44663</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3">
+        <v>1215</v>
+      </c>
+      <c r="G3">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44693</v>
+      </c>
+      <c r="C4">
+        <v>1219</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4">
+        <v>1215</v>
+      </c>
+      <c r="G4">
+        <v>1145</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1148,26 +858,583 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6D3776-44C9-402D-8899-CF36CF41AF68}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A26:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44758</v>
+      </c>
+      <c r="C3">
+        <v>1335</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44772</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44434</v>
+      </c>
+      <c r="C5">
+        <v>1010</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44483</v>
+      </c>
+      <c r="C6">
+        <v>1145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44519</v>
+      </c>
+      <c r="C7">
+        <v>1125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44547</v>
+      </c>
+      <c r="C8">
+        <v>1041</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44577</v>
+      </c>
+      <c r="C9">
+        <v>1150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44621</v>
+      </c>
+      <c r="C10">
+        <v>1250</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44658</v>
+      </c>
+      <c r="C11">
+        <v>1218</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44700</v>
+      </c>
+      <c r="C12">
+        <v>1015</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44742</v>
+      </c>
+      <c r="C13">
+        <v>910</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44775</v>
+      </c>
+      <c r="C14">
+        <v>1039</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1041</v>
+      </c>
+      <c r="G14">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44817</v>
+      </c>
+      <c r="C15">
+        <v>1145</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>1145</v>
+      </c>
+      <c r="G15">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44845</v>
+      </c>
+      <c r="C16">
+        <v>1204</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>1200</v>
+      </c>
+      <c r="G16">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44882</v>
+      </c>
+      <c r="C17">
+        <v>1401</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>1400</v>
+      </c>
+      <c r="G17">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44915</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>1245</v>
+      </c>
+      <c r="G18">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44959</v>
+      </c>
+      <c r="C19">
+        <v>1230</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19">
+        <v>1245</v>
+      </c>
+      <c r="G19">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45002</v>
+      </c>
+      <c r="C20">
+        <v>1218</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>1230</v>
+      </c>
+      <c r="G20">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45049</v>
+      </c>
+      <c r="C21">
+        <v>1317</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>1330</v>
+      </c>
+      <c r="G21">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45083</v>
+      </c>
+      <c r="C22">
+        <v>1044</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22">
+        <v>1200</v>
+      </c>
+      <c r="G22">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45120</v>
+      </c>
+      <c r="C23">
+        <v>1207</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>1215</v>
+      </c>
+      <c r="G23">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45147</v>
+      </c>
+      <c r="C24">
+        <v>1122</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="H26:I26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AA22A5-A68D-47B6-B1D8-BDBF4670AA92}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A21" sqref="A17:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1447,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1206,7 +1473,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1232,7 +1499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1255,7 +1522,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1278,7 +1545,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1301,7 +1568,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1324,7 +1591,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1347,7 +1614,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3">
         <v>44915</v>
@@ -1364,7 +1631,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1654,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1413,7 +1680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1437,7 +1704,7 @@
       </c>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1460,7 +1727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1483,7 +1750,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1497,61 +1764,108 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F002B337-BF1C-4A03-9136-9E55E40FA3F2}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:H27"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794A4FF-0009-47BD-A87F-C23E71CA6A9C}">
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1878,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1590,246 +1904,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1">
-        <v>44663</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>44782</v>
+      </c>
+      <c r="C3">
+        <v>1303</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" t="s">
         <v>51</v>
       </c>
       <c r="F3">
-        <v>1215</v>
-      </c>
-      <c r="G3">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44693</v>
-      </c>
-      <c r="C4">
-        <v>1219</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4">
-        <v>1215</v>
-      </c>
-      <c r="G4">
-        <v>1145</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794A4FF-0009-47BD-A87F-C23E71CA6A9C}">
-  <dimension ref="A1:H20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44782</v>
-      </c>
-      <c r="C3">
-        <v>1303</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3">
         <v>1330</v>
       </c>
       <c r="G3">
@@ -1839,7 +1930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1862,7 +1953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1885,7 +1976,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1908,7 +1999,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1929,7 +2020,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1952,7 +2043,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1975,7 +2066,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1998,7 +2089,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -2024,7 +2115,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2047,7 +2138,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2070,54 +2161,214 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1">
-        <v>45175</v>
-      </c>
-      <c r="C14">
-        <v>1004</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" s="1">
+        <v>45175</v>
+      </c>
+      <c r="C19">
+        <v>926</v>
+      </c>
+      <c r="D19">
+        <v>1004</v>
+      </c>
+      <c r="E19">
+        <v>1010</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19">
+        <v>1115</v>
+      </c>
+      <c r="I19">
+        <v>1215</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
+      <c r="B20" s="1">
+        <v>45223</v>
+      </c>
+      <c r="C20">
+        <v>1225</v>
+      </c>
+      <c r="D20">
+        <v>1251</v>
+      </c>
+      <c r="E20">
+        <v>1309</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20">
+        <v>1315</v>
+      </c>
+      <c r="I20">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45226</v>
+      </c>
+      <c r="C21">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>1100</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45244</v>
+      </c>
+      <c r="C22">
+        <v>1147</v>
+      </c>
+      <c r="D22">
+        <v>1238</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22">
+        <v>1315</v>
+      </c>
+      <c r="I22">
+        <v>915</v>
+      </c>
+      <c r="J22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45281</v>
+      </c>
+      <c r="C23">
+        <v>920</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="H17:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2126,23 +2377,24 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CD3886-B1BD-4EBA-ADC2-180D8A6D584C}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2155,7 +2407,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2181,7 +2433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -2202,7 +2454,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2228,7 +2480,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2254,7 +2506,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2277,7 +2529,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2300,7 +2552,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -2323,7 +2575,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2346,7 +2598,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -2369,7 +2621,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2395,7 +2647,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2418,7 +2670,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2441,7 +2693,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2464,7 +2716,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2487,7 +2739,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2513,43 +2765,195 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="1">
         <v>45152</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>1215</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>1315</v>
+      </c>
+      <c r="G17">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
+        <v>45194</v>
+      </c>
+      <c r="C21">
+        <v>1040</v>
+      </c>
+      <c r="D21">
+        <v>1110</v>
+      </c>
+      <c r="E21">
+        <v>1120</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21">
+        <v>1130</v>
+      </c>
+      <c r="I21">
+        <v>1030</v>
+      </c>
+      <c r="J21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
+      <c r="B22" s="1">
+        <v>45223</v>
+      </c>
+      <c r="C22">
+        <v>1034</v>
+      </c>
+      <c r="D22">
+        <v>1110</v>
+      </c>
+      <c r="E22">
+        <v>1117</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22">
+        <v>1130</v>
+      </c>
+      <c r="I22">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45258</v>
+      </c>
+      <c r="C23">
+        <v>1051</v>
+      </c>
+      <c r="D23">
+        <v>1120</v>
+      </c>
+      <c r="E23">
+        <v>1132</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23">
+        <v>1145</v>
+      </c>
+      <c r="I23">
+        <v>930</v>
+      </c>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44930</v>
+      </c>
+      <c r="C24">
+        <v>950</v>
+      </c>
+      <c r="D24">
+        <v>1013</v>
+      </c>
+      <c r="E24">
+        <v>1030</v>
+      </c>
+      <c r="F24" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="A19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2558,22 +2962,22 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E95F4B-5C9D-4198-986C-0225866E12A6}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2990,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +3016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2632,7 +3036,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2652,7 +3056,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2670,7 +3074,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2693,7 +3097,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2713,7 +3117,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2727,100 +3131,148 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2829,20 +3281,20 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D0DCC-8787-4FE7-BB99-C37778967274}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2855,7 +3307,7 @@
       </c>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2881,7 +3333,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2901,7 +3353,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2919,7 +3371,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2939,7 +3391,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2959,7 +3411,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2979,7 +3431,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2993,70 +3445,118 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="H11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3065,28 +3565,29 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16F255-BFBA-46FE-A8E9-25CFF9980EA9}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="A3" sqref="A3:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3097,55 +3598,177 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E61B50-78AE-4051-9DCA-CE85349BDC81}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAB0EEE-8947-4168-BA23-5BDB3B3C4A39}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection activeCell="A3" sqref="A3:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="H1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3156,25 +3779,126 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3447,7 +4171,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AA4D8C3-41DE-4DC8-A2DD-E94060DB3977}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AA4D8C3-41DE-4DC8-A2DD-E94060DB3977}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b86c8786-3949-4751-bfbd-0a78b1a1da57"/>
+    <ds:schemaRef ds:uri="b1310810-eaac-47f3-a903-b8b5d1f645b8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>